<commit_message>
updated func spec to reflect some of what we talked about in meeting.
</commit_message>
<xml_diff>
--- a/docs/functional-spec/GANTT_PROV_TIMELINE.xlsx
+++ b/docs/functional-spec/GANTT_PROV_TIMELINE.xlsx
@@ -915,6 +915,69 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="14" borderId="2" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="14" borderId="2" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="15" borderId="2" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="15" borderId="2" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -922,69 +985,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="14" borderId="2" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="14" borderId="2" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="15" borderId="2" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="15" borderId="2" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent5" xfId="13" builtinId="46"/>
@@ -1003,31 +1003,7 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1045,6 +1021,18 @@
           <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -1142,15 +1130,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="12"/>
-      <tableStyleElement type="headerRow" dxfId="11"/>
-      <tableStyleElement type="totalRow" dxfId="10"/>
-      <tableStyleElement type="firstColumn" dxfId="9"/>
-      <tableStyleElement type="lastColumn" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="secondRowStripe" dxfId="6"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="5"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="4"/>
+      <tableStyleElement type="wholeTable" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="10"/>
+      <tableStyleElement type="totalRow" dxfId="9"/>
+      <tableStyleElement type="firstColumn" dxfId="8"/>
+      <tableStyleElement type="lastColumn" dxfId="7"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="secondRowStripe" dxfId="5"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1568,8 +1556,8 @@
   <dimension ref="A1:BL41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F42" sqref="F42"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1614,15 +1602,15 @@
       <c r="B3" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="C3" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="77"/>
-      <c r="E3" s="82">
+      <c r="D3" s="98"/>
+      <c r="E3" s="96">
         <f ca="1">TODAY()</f>
-        <v>43784</v>
-      </c>
-      <c r="F3" s="82"/>
+        <v>43787</v>
+      </c>
+      <c r="F3" s="96"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
@@ -1631,327 +1619,327 @@
       <c r="B4" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="77"/>
+      <c r="D4" s="98"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="79">
+      <c r="I4" s="93">
         <f ca="1">I5</f>
-        <v>43780</v>
-      </c>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="79">
+        <v>43787</v>
+      </c>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="93">
         <f ca="1">P5</f>
-        <v>43787</v>
-      </c>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="80"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="79">
+        <v>43794</v>
+      </c>
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="94"/>
+      <c r="T4" s="94"/>
+      <c r="U4" s="94"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="93">
         <f ca="1">W5</f>
-        <v>43794</v>
-      </c>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="80"/>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="79">
+        <v>43801</v>
+      </c>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="95"/>
+      <c r="AD4" s="93">
         <f ca="1">AD5</f>
-        <v>43801</v>
-      </c>
-      <c r="AE4" s="80"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="80"/>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="80"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="79">
+        <v>43808</v>
+      </c>
+      <c r="AE4" s="94"/>
+      <c r="AF4" s="94"/>
+      <c r="AG4" s="94"/>
+      <c r="AH4" s="94"/>
+      <c r="AI4" s="94"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="93">
         <f ca="1">AK5</f>
-        <v>43808</v>
-      </c>
-      <c r="AL4" s="80"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="80"/>
-      <c r="AO4" s="80"/>
-      <c r="AP4" s="80"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="79">
+        <v>43815</v>
+      </c>
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
+      <c r="AN4" s="94"/>
+      <c r="AO4" s="94"/>
+      <c r="AP4" s="94"/>
+      <c r="AQ4" s="95"/>
+      <c r="AR4" s="93">
         <f ca="1">AR5</f>
-        <v>43815</v>
-      </c>
-      <c r="AS4" s="80"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="80"/>
-      <c r="AV4" s="80"/>
-      <c r="AW4" s="80"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="79">
+        <v>43822</v>
+      </c>
+      <c r="AS4" s="94"/>
+      <c r="AT4" s="94"/>
+      <c r="AU4" s="94"/>
+      <c r="AV4" s="94"/>
+      <c r="AW4" s="94"/>
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="93">
         <f ca="1">AY5</f>
-        <v>43822</v>
-      </c>
-      <c r="AZ4" s="80"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="80"/>
-      <c r="BC4" s="80"/>
-      <c r="BD4" s="80"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="79">
+        <v>43829</v>
+      </c>
+      <c r="AZ4" s="94"/>
+      <c r="BA4" s="94"/>
+      <c r="BB4" s="94"/>
+      <c r="BC4" s="94"/>
+      <c r="BD4" s="94"/>
+      <c r="BE4" s="95"/>
+      <c r="BF4" s="93">
         <f ca="1">BF5</f>
-        <v>43829</v>
-      </c>
-      <c r="BG4" s="80"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="80"/>
-      <c r="BJ4" s="80"/>
-      <c r="BK4" s="80"/>
-      <c r="BL4" s="81"/>
+        <v>43836</v>
+      </c>
+      <c r="BG4" s="94"/>
+      <c r="BH4" s="94"/>
+      <c r="BI4" s="94"/>
+      <c r="BJ4" s="94"/>
+      <c r="BK4" s="94"/>
+      <c r="BL4" s="95"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>43780</v>
+        <v>43787</v>
       </c>
       <c r="J5" s="10">
         <f ca="1">I5+1</f>
-        <v>43781</v>
+        <v>43788</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>43782</v>
+        <v>43789</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43783</v>
+        <v>43790</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43784</v>
+        <v>43791</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43785</v>
+        <v>43792</v>
       </c>
       <c r="O5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43786</v>
+        <v>43793</v>
       </c>
       <c r="P5" s="11">
         <f ca="1">O5+1</f>
-        <v>43787</v>
+        <v>43794</v>
       </c>
       <c r="Q5" s="10">
         <f ca="1">P5+1</f>
-        <v>43788</v>
+        <v>43795</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43789</v>
+        <v>43796</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43790</v>
+        <v>43797</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43791</v>
+        <v>43798</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43792</v>
+        <v>43799</v>
       </c>
       <c r="V5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43793</v>
+        <v>43800</v>
       </c>
       <c r="W5" s="11">
         <f ca="1">V5+1</f>
-        <v>43794</v>
+        <v>43801</v>
       </c>
       <c r="X5" s="10">
         <f ca="1">W5+1</f>
-        <v>43795</v>
+        <v>43802</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43796</v>
+        <v>43803</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43797</v>
+        <v>43804</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43798</v>
+        <v>43805</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43799</v>
+        <v>43806</v>
       </c>
       <c r="AC5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43800</v>
+        <v>43807</v>
       </c>
       <c r="AD5" s="11">
         <f ca="1">AC5+1</f>
-        <v>43801</v>
+        <v>43808</v>
       </c>
       <c r="AE5" s="10">
         <f ca="1">AD5+1</f>
-        <v>43802</v>
+        <v>43809</v>
       </c>
       <c r="AF5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43803</v>
+        <v>43810</v>
       </c>
       <c r="AG5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43804</v>
+        <v>43811</v>
       </c>
       <c r="AH5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43805</v>
+        <v>43812</v>
       </c>
       <c r="AI5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43806</v>
+        <v>43813</v>
       </c>
       <c r="AJ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43807</v>
+        <v>43814</v>
       </c>
       <c r="AK5" s="11">
         <f ca="1">AJ5+1</f>
-        <v>43808</v>
+        <v>43815</v>
       </c>
       <c r="AL5" s="10">
         <f ca="1">AK5+1</f>
-        <v>43809</v>
+        <v>43816</v>
       </c>
       <c r="AM5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43810</v>
+        <v>43817</v>
       </c>
       <c r="AN5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43811</v>
+        <v>43818</v>
       </c>
       <c r="AO5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43812</v>
+        <v>43819</v>
       </c>
       <c r="AP5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43813</v>
+        <v>43820</v>
       </c>
       <c r="AQ5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43814</v>
+        <v>43821</v>
       </c>
       <c r="AR5" s="11">
         <f ca="1">AQ5+1</f>
-        <v>43815</v>
+        <v>43822</v>
       </c>
       <c r="AS5" s="10">
         <f ca="1">AR5+1</f>
-        <v>43816</v>
+        <v>43823</v>
       </c>
       <c r="AT5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43817</v>
+        <v>43824</v>
       </c>
       <c r="AU5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43818</v>
+        <v>43825</v>
       </c>
       <c r="AV5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43819</v>
+        <v>43826</v>
       </c>
       <c r="AW5" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>43820</v>
+        <v>43827</v>
       </c>
       <c r="AX5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>43821</v>
+        <v>43828</v>
       </c>
       <c r="AY5" s="11">
         <f ca="1">AX5+1</f>
-        <v>43822</v>
+        <v>43829</v>
       </c>
       <c r="AZ5" s="10">
         <f ca="1">AY5+1</f>
-        <v>43823</v>
+        <v>43830</v>
       </c>
       <c r="BA5" s="10">
         <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>43824</v>
+        <v>43831</v>
       </c>
       <c r="BB5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43825</v>
+        <v>43832</v>
       </c>
       <c r="BC5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43826</v>
+        <v>43833</v>
       </c>
       <c r="BD5" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>43827</v>
+        <v>43834</v>
       </c>
       <c r="BE5" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>43828</v>
+        <v>43835</v>
       </c>
       <c r="BF5" s="11">
         <f ca="1">BE5+1</f>
-        <v>43829</v>
+        <v>43836</v>
       </c>
       <c r="BG5" s="10">
         <f ca="1">BF5+1</f>
-        <v>43830</v>
+        <v>43837</v>
       </c>
       <c r="BH5" s="10">
         <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>43831</v>
+        <v>43838</v>
       </c>
       <c r="BI5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43832</v>
+        <v>43839</v>
       </c>
       <c r="BJ5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43833</v>
+        <v>43840</v>
       </c>
       <c r="BK5" s="10">
         <f t="shared" ca="1" si="2"/>
-        <v>43834</v>
+        <v>43841</v>
       </c>
       <c r="BL5" s="12">
         <f t="shared" ca="1" si="2"/>
-        <v>43835</v>
+        <v>43842</v>
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2122,7 +2110,7 @@
         <v>M</v>
       </c>
       <c r="AS6" s="13" t="str">
-        <f t="shared" ref="AS6:CV6" ca="1" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
+        <f t="shared" ref="AS6:BL6" ca="1" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="AT6" s="13" t="str">
@@ -2346,10 +2334,10 @@
       <c r="A9" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="90" t="s">
+      <c r="C9" s="83" t="s">
         <v>50</v>
       </c>
       <c r="D9" s="21">
@@ -2357,7 +2345,7 @@
       </c>
       <c r="E9" s="65">
         <f ca="1">Project_Start</f>
-        <v>43784</v>
+        <v>43787</v>
       </c>
       <c r="F9" s="65">
         <v>43873</v>
@@ -2365,7 +2353,7 @@
       <c r="G9" s="16"/>
       <c r="H9" s="16">
         <f t="shared" ca="1" si="6"/>
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -2428,10 +2416,10 @@
       <c r="A10" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="95" t="s">
+      <c r="B10" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="83" t="s">
         <v>50</v>
       </c>
       <c r="D10" s="21">
@@ -2507,10 +2495,10 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="57"/>
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="83" t="s">
         <v>50</v>
       </c>
       <c r="D11" s="21">
@@ -2586,10 +2574,10 @@
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="57"/>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="83" t="s">
         <v>50</v>
       </c>
       <c r="D12" s="21">
@@ -2666,10 +2654,10 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="57"/>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="88" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="90" t="s">
+      <c r="C13" s="83" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="21">
@@ -2819,10 +2807,10 @@
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="58"/>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="84" t="s">
         <v>51</v>
       </c>
       <c r="D15" s="26">
@@ -2900,10 +2888,10 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="57"/>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="91" t="s">
+      <c r="C16" s="84" t="s">
         <v>51</v>
       </c>
       <c r="D16" s="26">
@@ -2984,7 +2972,7 @@
       <c r="B17" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="91" t="s">
+      <c r="C17" s="84" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="26"/>
@@ -3063,7 +3051,7 @@
       <c r="B18" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="91" t="s">
+      <c r="C18" s="84" t="s">
         <v>51</v>
       </c>
       <c r="D18" s="26"/>
@@ -3142,7 +3130,7 @@
       <c r="B19" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="91" t="s">
+      <c r="C19" s="84" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="26"/>
@@ -3291,20 +3279,20 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="57"/>
-      <c r="B21" s="97" t="s">
+      <c r="B21" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="92" t="s">
+      <c r="C21" s="85" t="s">
         <v>52</v>
       </c>
       <c r="D21" s="31"/>
       <c r="E21" s="67">
         <f ca="1">E9+15</f>
-        <v>43799</v>
+        <v>43802</v>
       </c>
       <c r="F21" s="67">
         <f ca="1">E21+5</f>
-        <v>43804</v>
+        <v>43807</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="16">
@@ -3370,20 +3358,20 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="57"/>
-      <c r="B22" s="97" t="s">
+      <c r="B22" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="92" t="s">
+      <c r="C22" s="85" t="s">
         <v>52</v>
       </c>
       <c r="D22" s="31"/>
       <c r="E22" s="67">
         <f ca="1">F21+1</f>
-        <v>43805</v>
+        <v>43808</v>
       </c>
       <c r="F22" s="67">
         <f ca="1">E22+4</f>
-        <v>43809</v>
+        <v>43812</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16">
@@ -3452,17 +3440,17 @@
       <c r="B23" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="92" t="s">
+      <c r="C23" s="85" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="31"/>
       <c r="E23" s="67">
         <f ca="1">E22+5</f>
-        <v>43810</v>
+        <v>43813</v>
       </c>
       <c r="F23" s="67">
         <f ca="1">E23+5</f>
-        <v>43815</v>
+        <v>43818</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="16">
@@ -3531,17 +3519,17 @@
       <c r="B24" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="92" t="s">
+      <c r="C24" s="85" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="31"/>
       <c r="E24" s="67">
         <f ca="1">F23+1</f>
-        <v>43816</v>
+        <v>43819</v>
       </c>
       <c r="F24" s="67">
         <f ca="1">E24+4</f>
-        <v>43820</v>
+        <v>43823</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="16">
@@ -3610,17 +3598,17 @@
       <c r="B25" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="92" t="s">
+      <c r="C25" s="85" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="31"/>
       <c r="E25" s="67">
         <f ca="1">E23</f>
-        <v>43810</v>
+        <v>43813</v>
       </c>
       <c r="F25" s="67">
         <f ca="1">E25+4</f>
-        <v>43814</v>
+        <v>43817</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16">
@@ -3759,10 +3747,10 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="57"/>
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="91" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="93" t="s">
+      <c r="C27" s="86" t="s">
         <v>52</v>
       </c>
       <c r="D27" s="36"/>
@@ -3836,10 +3824,10 @@
     </row>
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="57"/>
-      <c r="B28" s="98" t="s">
+      <c r="B28" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="93" t="s">
+      <c r="C28" s="86" t="s">
         <v>52</v>
       </c>
       <c r="D28" s="36"/>
@@ -3916,7 +3904,7 @@
       <c r="B29" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="93" t="s">
+      <c r="C29" s="86" t="s">
         <v>52</v>
       </c>
       <c r="D29" s="36"/>
@@ -3993,7 +3981,7 @@
       <c r="B30" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="93" t="s">
+      <c r="C30" s="86" t="s">
         <v>52</v>
       </c>
       <c r="D30" s="36"/>
@@ -4070,7 +4058,7 @@
       <c r="B31" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="93" t="s">
+      <c r="C31" s="86" t="s">
         <v>52</v>
       </c>
       <c r="D31" s="36"/>
@@ -4146,13 +4134,13 @@
       <c r="A32" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="83" t="s">
+      <c r="B32" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="86"/>
-      <c r="D32" s="87"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="81"/>
       <c r="G32" s="16"/>
       <c r="H32" s="16" t="str">
         <f t="shared" si="6"/>
@@ -4217,17 +4205,17 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="57"/>
-      <c r="B33" s="99" t="s">
+      <c r="B33" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="94" t="s">
+      <c r="C33" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="D33" s="84"/>
-      <c r="E33" s="85">
+      <c r="D33" s="77"/>
+      <c r="E33" s="78">
         <v>43770</v>
       </c>
-      <c r="F33" s="85">
+      <c r="F33" s="78">
         <v>43791</v>
       </c>
       <c r="G33" s="16"/>
@@ -4291,17 +4279,17 @@
     </row>
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="57"/>
-      <c r="B34" s="99" t="s">
+      <c r="B34" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="94" t="s">
+      <c r="C34" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="D34" s="84"/>
-      <c r="E34" s="85" t="s">
+      <c r="D34" s="77"/>
+      <c r="E34" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="85" t="s">
+      <c r="F34" s="78" t="s">
         <v>28</v>
       </c>
       <c r="G34" s="16"/>
@@ -4365,17 +4353,17 @@
     </row>
     <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="57"/>
-      <c r="B35" s="99" t="s">
+      <c r="B35" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="94" t="s">
+      <c r="C35" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="84"/>
-      <c r="E35" s="85">
+      <c r="D35" s="77"/>
+      <c r="E35" s="78">
         <v>43956</v>
       </c>
-      <c r="F35" s="85">
+      <c r="F35" s="78">
         <v>43962</v>
       </c>
       <c r="G35" s="16"/>
@@ -4439,17 +4427,17 @@
     </row>
     <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="57"/>
-      <c r="B36" s="89" t="s">
+      <c r="B36" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="94" t="s">
+      <c r="C36" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="84"/>
-      <c r="E36" s="85" t="s">
+      <c r="D36" s="77"/>
+      <c r="E36" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="F36" s="85" t="s">
+      <c r="F36" s="78" t="s">
         <v>28</v>
       </c>
       <c r="G36" s="16"/>
@@ -4513,17 +4501,17 @@
     </row>
     <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="57"/>
-      <c r="B37" s="89" t="s">
+      <c r="B37" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="94" t="s">
+      <c r="C37" s="87" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="84"/>
-      <c r="E37" s="85" t="s">
+      <c r="D37" s="77"/>
+      <c r="E37" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="85" t="s">
+      <c r="F37" s="78" t="s">
         <v>28</v>
       </c>
       <c r="G37" s="16"/>
@@ -4670,6 +4658,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4677,11 +4670,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D31 D38">
     <cfRule type="dataBar" priority="15">
@@ -4698,15 +4686,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:BL38">
-    <cfRule type="expression" dxfId="1" priority="34">
+    <cfRule type="expression" dxfId="2" priority="34">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:BL38">
-    <cfRule type="expression" dxfId="3" priority="28">
+    <cfRule type="expression" dxfId="1" priority="28">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="29" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>